<commit_message>
added compounds cluster html file
</commit_message>
<xml_diff>
--- a/results/clusters.xlsx
+++ b/results/clusters.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Diethyl maleate</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -458,7 +458,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Triamcinolone acetonide</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -468,7 +468,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -478,7 +478,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -488,7 +488,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -498,7 +498,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Betamethasone-17-valerate</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -508,7 +508,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Hydrocortisone-21-hemisuccinate</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -518,7 +518,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -528,7 +528,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -538,7 +538,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Triamcinolone acetonide</t>
+          <t>Heptanol</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -548,7 +548,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Heptanol</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -558,7 +558,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>n-heptanol</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -568,7 +568,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -578,7 +578,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Diethylene glycol monobutyl ether</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -588,7 +588,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Diethylene glycol monobutyl ether</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -598,7 +598,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t xml:space="preserve">Decanol </t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -608,7 +608,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>n-decanol</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -618,7 +618,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Decanol</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -628,7 +628,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Hydroxypregnenolone</t>
+          <t>decanol</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -638,7 +638,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Pregnenolone</t>
+          <t>n-propanol</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -648,7 +648,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Hydrocortisone</t>
+          <t>2,3-Butanediol</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -658,7 +658,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Hydrocortisone</t>
+          <t>decanol</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -668,7 +668,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hydrocortisone </t>
+          <t>Propanol</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -678,7 +678,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hydrocortisone </t>
+          <t>2-Butanone</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -688,7 +688,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Butanol</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -698,7 +698,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>n-nonanol</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -708,7 +708,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Nonanol</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -718,7 +718,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Butanol</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -728,7 +728,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Diethyl maleate</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -738,7 +738,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>acetic acid</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -748,7 +748,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Butanol</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -758,7 +758,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Butanol</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -768,7 +768,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>n-butanol</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -778,7 +778,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Butanol</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -788,7 +788,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Pentanol</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -798,7 +798,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>n-pentanol</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -808,7 +808,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>acetic acid</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -818,7 +818,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Triamcinolone</t>
+          <t>acetic acid</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -828,7 +828,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>acetic acid</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -838,7 +838,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Ethanol</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -848,7 +848,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>ethanol</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -858,7 +858,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Ethanol</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -868,7 +868,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Methylglucose</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -878,7 +878,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Propanol</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -888,7 +888,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>decanol</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -898,7 +898,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>decanol</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -908,7 +908,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Decanol</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -918,7 +918,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Urea</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -928,7 +928,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Urea</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -938,7 +938,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Urea</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -948,7 +948,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Urea</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -958,7 +958,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>urea</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -968,7 +968,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>urea</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -978,7 +978,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -988,7 +988,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -998,7 +998,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>decanol</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1008,7 +1008,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Ethyl ether</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1018,7 +1018,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Geraniol</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1028,7 +1028,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>methanol</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1038,7 +1038,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Methanol</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1048,7 +1048,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Methanol</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1058,7 +1058,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>17-alfa-Hydroxyprogesterone</t>
+          <t>Methyl methanesulfonate</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1068,7 +1068,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Hydrocortisone-21-propionate</t>
+          <t>2-Ethylhexyl acrylate</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1078,7 +1078,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>2-Ethylhexyl acrylate</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1088,7 +1088,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Methyl methanesulfonate</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1098,7 +1098,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Geraniol</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1108,7 +1108,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Hydrocortisone-21-hexanoate; Hydrocortisone caproate</t>
+          <t>Urea</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1118,7 +1118,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Cortexone</t>
+          <t>acetic acid</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1128,7 +1128,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>n-hexanol</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1138,7 +1138,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Octanol</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1148,7 +1148,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>butoxyethanol</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1158,7 +1158,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Dexamethasone</t>
+          <t>butoxyethanol</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1168,7 +1168,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>butoxyethanol</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1178,7 +1178,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>butoxyethanol</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1188,7 +1188,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>n-octanol</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1198,7 +1198,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>butoxyethanol</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1208,7 +1208,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Corticosterone</t>
+          <t>Hexanol</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1218,7 +1218,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Hydrocortisone</t>
+          <t>Octanol</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1228,7 +1228,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Prednisolone</t>
+          <t>Octanol</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1238,7 +1238,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>testosterone</t>
+          <t>2-Ethoxy ethanol</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1248,7 +1248,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Testosterone</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1258,7 +1258,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Testosterone</t>
+          <t>Mannitol</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1268,7 +1268,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Hydrocortisone</t>
+          <t>Octanol</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1278,7 +1278,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Raffinose</t>
+          <t>Glycerol</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1288,7 +1288,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Raffinose</t>
+          <t>Glycerol</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1298,7 +1298,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Progesterone</t>
+          <t>Hexanol</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -1308,141 +1308,141 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Progesterone</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Aldosterone</t>
+          <t>Cortexone</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Aldosterone</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Aldosterone</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Aldosterone</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Aldosterone</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Aldosterone</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Cortisone</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>cortisone</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Progesterone</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Progesterone</t>
+          <t>Beta-estradiol</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Progesterone</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>testosterone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>testosterone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -1452,133 +1452,133 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>testosterone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>testosterone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Testosterone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Testosterone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Testosterone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>testosterone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Testosterone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Testosterone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Testosterone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Testosterone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Testosterone</t>
+          <t xml:space="preserve">Hydrocortisone </t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Testosterone</t>
+          <t xml:space="preserve">Hydrocortisone </t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Hydrocortisone</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -1588,7 +1588,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Hydrocortisone</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -1598,7 +1598,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -1608,7 +1608,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Chlorocresol</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -1618,7 +1618,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>chlorocresol</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -1628,7 +1628,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>beta-Estradiol</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -1638,7 +1638,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2-Phenylethanol</t>
+          <t>Beta-estradiol</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -1648,7 +1648,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2-phenylethanol</t>
+          <t>beta-Estradiol</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -1658,7 +1658,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>4-Amino-3-nitrophenol</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -1668,7 +1668,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>4-Amino-3-nitrophenol</t>
+          <t>beta-Estradiol</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -1678,7 +1678,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Nicotinate, ethyl</t>
+          <t>beta-Estradiol</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -1688,7 +1688,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Nicotinate, ethyl</t>
+          <t>Estriol</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -1698,7 +1698,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>1,2,4-Benzenetriol</t>
+          <t>Estriol</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -1708,7 +1708,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>4-Hydroxybenzyl alcohol</t>
+          <t>Prednisolone</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -1718,7 +1718,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>m-Nitrophenol; 3-nitrophenol</t>
+          <t>Hydrocortisone</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -1728,7 +1728,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>chlorocresol</t>
+          <t>Hydrocortisone</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -1738,7 +1738,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -1748,7 +1748,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -1758,7 +1758,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -1768,7 +1768,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Caffeine</t>
+          <t>Beta-Estradiol</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -1778,7 +1778,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Caffeine</t>
+          <t>Estrone</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -1788,7 +1788,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Caffeine</t>
+          <t>Estrone</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -1798,7 +1798,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Caffeine</t>
+          <t>Testosterone</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -1808,7 +1808,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>caffeine</t>
+          <t>Testosterone</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -1818,7 +1818,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Caffeine</t>
+          <t>Testosterone</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -1828,7 +1828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Caffeine</t>
+          <t>Testosterone</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -1838,7 +1838,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>5-Fluorouracil (+ - + -)</t>
+          <t>testosterone</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -1848,7 +1848,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>testosterone</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -1858,7 +1858,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>testosterone</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -1868,7 +1868,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>testosterone</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -1878,7 +1878,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>testosterone</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -1888,7 +1888,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>testosterone</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -1898,7 +1898,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Testosterone</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -1908,7 +1908,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Testosterone</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -1918,7 +1918,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Progesterone</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -1928,7 +1928,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Progesterone</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -1938,7 +1938,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Progesterone</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -1948,7 +1948,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Progesterone</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -1958,7 +1958,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Progesterone</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -1968,7 +1968,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>cortisone</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -1978,7 +1978,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Cortisone</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -1988,7 +1988,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>5-Fluorouracil</t>
+          <t>Aldosterone</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -1998,7 +1998,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>p-Nitrophenol; 4-nitrophenol</t>
+          <t>Aldosterone</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -2008,7 +2008,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Iso-thymol; Carvacrol</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -2018,7 +2018,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Isoeugenol</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -2028,7 +2028,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Isoeugenol</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -2038,7 +2038,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Eugenol</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -2048,7 +2048,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Eugenol</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -2058,7 +2058,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2,4-Dinitrochlorobenzene</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -2068,7 +2068,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2,4-Dinitrochlorobenzene</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -2078,7 +2078,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>3,4-Xylenol</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -2088,7 +2088,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>o-Chlorophenol</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -2098,7 +2098,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>o-Phenylenediamine</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -2108,7 +2108,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>o-Cresol</t>
+          <t>Estradiol</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -2118,7 +2118,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Butylparaben</t>
+          <t>Testosterone</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -2128,7 +2128,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Butylparaben</t>
+          <t>Testosterone</t>
         </is>
       </c>
       <c r="B170" t="n">
@@ -2138,7 +2138,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Acetophenone</t>
+          <t>Testosterone</t>
         </is>
       </c>
       <c r="B171" t="n">
@@ -2148,7 +2148,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Propylparaben</t>
+          <t>Testosterone</t>
         </is>
       </c>
       <c r="B172" t="n">
@@ -2158,7 +2158,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>propylparaben</t>
+          <t>Testosterone</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -2168,7 +2168,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>propylparaben</t>
+          <t>Aldosterone</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -2178,7 +2178,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>propylparaben</t>
+          <t>Aldosterone</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -2188,7 +2188,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>propylparaben</t>
+          <t>Aldosterone</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -2198,7 +2198,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>propylparaben</t>
+          <t>Aldosterone</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -2208,7 +2208,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>propylparaben</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -2218,7 +2218,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2,4-Dichloroacetophenone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -2228,7 +2228,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2,4-Dichloroacetophenone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B180" t="n">
@@ -2238,7 +2238,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Nicotinate, methyl</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B181" t="n">
@@ -2248,7 +2248,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>4-Amino-2-Nitrophenol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B182" t="n">
@@ -2258,7 +2258,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>methyl salicylate</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B183" t="n">
@@ -2268,7 +2268,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Benzophenone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B184" t="n">
@@ -2278,7 +2278,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Propylparaben</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B185" t="n">
@@ -2288,7 +2288,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>catechol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -2298,7 +2298,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Acetophenone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B187" t="n">
@@ -2308,7 +2308,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Methylparaben</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -2318,7 +2318,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Benzyl bromide</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B189" t="n">
@@ -2328,7 +2328,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Benzyl bromide</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B190" t="n">
@@ -2338,7 +2338,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Benzyl alcohol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B191" t="n">
@@ -2348,7 +2348,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Cinnamyl alcohol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B192" t="n">
@@ -2358,7 +2358,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Cinnamyl alcohol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -2368,7 +2368,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>p-Tolunitrile</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -2378,7 +2378,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>p-Tolunitrile</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -2388,7 +2388,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>5-phenylpentanol</t>
+          <t>Dexamethasone</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -2398,7 +2398,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Methylparaben</t>
+          <t>Hydrocortisone-21-propionate</t>
         </is>
       </c>
       <c r="B197" t="n">
@@ -2408,7 +2408,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Methylparaben</t>
+          <t>17-alfa-Hydroxyprogesterone</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -2418,7 +2418,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>p-Bromophenol</t>
+          <t>Hydrocortisone-21-hexanoate; Hydrocortisone caproate</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -2428,7 +2428,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>p-Cresol</t>
+          <t>Hydrocortisone-21-hemisuccinate</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -2438,7 +2438,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Methylparaben</t>
+          <t>Betamethasone-17-valerate</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -2448,7 +2448,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>p-Cresol</t>
+          <t>Naltrexone</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -2458,7 +2458,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>p-Phenylenediamine</t>
+          <t>Hydroxypregnenolone</t>
         </is>
       </c>
       <c r="B203" t="n">
@@ -2468,7 +2468,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>m-Cresol</t>
+          <t>Pregnenolone</t>
         </is>
       </c>
       <c r="B204" t="n">
@@ -2478,7 +2478,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Resorcinol; 1,3-Benzenediol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -2488,7 +2488,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>resorcinol</t>
+          <t>Triamcinolone acetonide</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -2498,7 +2498,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Resorcinol</t>
+          <t>Triamcinolone acetonide</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -2508,7 +2508,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Resorcinol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B208" t="n">
@@ -2518,7 +2518,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>phloroglucinol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B209" t="n">
@@ -2528,7 +2528,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Toluene</t>
+          <t>Triamcinolone</t>
         </is>
       </c>
       <c r="B210" t="n">
@@ -2538,7 +2538,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Phenol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B211" t="n">
@@ -2548,7 +2548,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Phenol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B212" t="n">
@@ -2558,7 +2558,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Phenol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B213" t="n">
@@ -2568,7 +2568,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B214" t="n">
@@ -2578,7 +2578,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>p-Chlorophenol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B215" t="n">
@@ -2588,7 +2588,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2,4-Dichlorophenol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B216" t="n">
@@ -2598,7 +2598,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Benzophenone</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B217" t="n">
@@ -2608,7 +2608,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2,4-dichlorophenol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B218" t="n">
@@ -2618,7 +2618,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>pyrogallol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B219" t="n">
@@ -2628,7 +2628,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2,4-dichlorophenol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B220" t="n">
@@ -2638,7 +2638,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>trans-Cinnamaldehyde</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B221" t="n">
@@ -2648,7 +2648,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Diethyl phthalate</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B222" t="n">
@@ -2658,7 +2658,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>p-n-butylphenol; 4-Butylphenol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B223" t="n">
@@ -2668,7 +2668,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>alfa-(4-Hydroxyphenyl) acetamide</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B224" t="n">
@@ -2678,7 +2678,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>4-propoxyphenol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B225" t="n">
@@ -2688,7 +2688,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>4-propoxyphenol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B226" t="n">
@@ -2698,7 +2698,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>4-Bromophenyl isocyanate</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B227" t="n">
@@ -2708,7 +2708,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>4-Bromophenyl isocyanate</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B228" t="n">
@@ -2718,7 +2718,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>3-Methyl-3H-imidazo[4,5-f]quinolin-2-amine</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B229" t="n">
@@ -2728,7 +2728,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>HC Red No. 3; 2-(4-Amino-2-nitroanilino)-ethanol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B230" t="n">
@@ -2738,7 +2738,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>HC Red No. 3; 2-(4-Amino-2-nitroanilino)-ethanol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B231" t="n">
@@ -2748,7 +2748,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>3-Methyl-3H-imidazo[4,5-f]quinolin-2-amine</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B232" t="n">
@@ -2758,7 +2758,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>7-Ethoxycoumarin</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B233" t="n">
@@ -2768,7 +2768,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>7-Ethoxycoumarin</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B234" t="n">
@@ -2778,7 +2778,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Benzene</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B235" t="n">
@@ -2788,7 +2788,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>4-phenylbutanol</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B236" t="n">
@@ -2798,7 +2798,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Benzene</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B237" t="n">
@@ -2808,7 +2808,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Salicylic acid</t>
+          <t>Corticosterone</t>
         </is>
       </c>
       <c r="B238" t="n">
@@ -2818,357 +2818,357 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Salicylic acid</t>
+          <t>Propylparaben</t>
         </is>
       </c>
       <c r="B239" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>benzoic acid</t>
+          <t>Propylparaben</t>
         </is>
       </c>
       <c r="B240" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>Benzoic acid</t>
+          <t>propylparaben</t>
         </is>
       </c>
       <c r="B241" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Benzoic acid</t>
+          <t>Nicotinate, methyl</t>
         </is>
       </c>
       <c r="B242" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>salicylate</t>
+          <t>2,4-Dichloroacetophenone</t>
         </is>
       </c>
       <c r="B243" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>salicylate</t>
+          <t>propylparaben</t>
         </is>
       </c>
       <c r="B244" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>salicylate</t>
+          <t>propylparaben</t>
         </is>
       </c>
       <c r="B245" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Chloroxylenol</t>
+          <t>propylparaben</t>
         </is>
       </c>
       <c r="B246" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Methyl 4-hydroxyphenylacetate</t>
+          <t>2,4-Dichloroacetophenone</t>
         </is>
       </c>
       <c r="B247" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>trans-Cinnamaldehyde</t>
+          <t>Butylparaben</t>
         </is>
       </c>
       <c r="B248" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2,4,6-Trichlorophenol</t>
+          <t>propylparaben</t>
         </is>
       </c>
       <c r="B249" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2,4-dichlorophenol</t>
+          <t>propylparaben</t>
         </is>
       </c>
       <c r="B250" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2,4-dichlorophenol</t>
+          <t>Nicotinate, methyl</t>
         </is>
       </c>
       <c r="B251" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Nicotinate, methyl</t>
+          <t>Butylparaben</t>
         </is>
       </c>
       <c r="B252" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>6-Methylcoumarin</t>
+          <t>Acetophenone</t>
         </is>
       </c>
       <c r="B253" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>6-Methylcoumarin</t>
+          <t>o-Phenylenediamine</t>
         </is>
       </c>
       <c r="B254" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>chloroxylenol</t>
+          <t>Caffeine</t>
         </is>
       </c>
       <c r="B255" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Naphthalene</t>
+          <t>Methylparaben</t>
         </is>
       </c>
       <c r="B256" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>Benzylideneacetone</t>
+          <t>Methylparaben</t>
         </is>
       </c>
       <c r="B257" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Benzylideneacetone</t>
+          <t>Methylparaben</t>
         </is>
       </c>
       <c r="B258" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>p-Ethylphenol</t>
+          <t>Methylparaben</t>
         </is>
       </c>
       <c r="B259" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Hydroquinone</t>
+          <t>Acetophenone</t>
         </is>
       </c>
       <c r="B260" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Naphthalene</t>
+          <t>6-Methylcoumarin</t>
         </is>
       </c>
       <c r="B261" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Hydroquinone</t>
+          <t>Isoeugenol</t>
         </is>
       </c>
       <c r="B262" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Hydroquinone</t>
+          <t>Isoeugenol</t>
         </is>
       </c>
       <c r="B263" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Dimethyl phthalate</t>
+          <t>Eugenol</t>
         </is>
       </c>
       <c r="B264" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>Dimethyl phthalate</t>
+          <t>Eugenol</t>
         </is>
       </c>
       <c r="B265" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>Beta-naphthol; 2-naphthol</t>
+          <t>2,4-Dinitrochlorobenzene</t>
         </is>
       </c>
       <c r="B266" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>Beta-naphthol; 2-naphthol</t>
+          <t>2,4-Dinitrochlorobenzene</t>
         </is>
       </c>
       <c r="B267" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>Naphthol</t>
+          <t>3,4-Xylenol</t>
         </is>
       </c>
       <c r="B268" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>Naphthol</t>
+          <t>o-Chlorophenol</t>
         </is>
       </c>
       <c r="B269" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>Thymol; 2-Isopropyl-5-methylphenol</t>
+          <t>o-Cresol</t>
         </is>
       </c>
       <c r="B270" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Thymol; 2-Isopropyl-5-methylphenol</t>
+          <t>6-Methylcoumarin</t>
         </is>
       </c>
       <c r="B271" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>hydroquinone</t>
+          <t>Chlorocresol</t>
         </is>
       </c>
       <c r="B272" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>o-t-butylphenol</t>
+          <t>Naphthalene</t>
         </is>
       </c>
       <c r="B273" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Sucrose</t>
+          <t>4-Hydroxybenzyl alcohol</t>
         </is>
       </c>
       <c r="B274" t="n">
@@ -3178,7 +3178,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>Sucrose</t>
+          <t>salicylate</t>
         </is>
       </c>
       <c r="B275" t="n">
@@ -3188,7 +3188,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>Sucrose</t>
+          <t>salicylate</t>
         </is>
       </c>
       <c r="B276" t="n">
@@ -3198,7 +3198,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>sucrose</t>
+          <t>salicylate</t>
         </is>
       </c>
       <c r="B277" t="n">
@@ -3208,7 +3208,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>Methotrexate</t>
+          <t>3-Methyl-3H-imidazo[4,5-f]quinolin-2-amine</t>
         </is>
       </c>
       <c r="B278" t="n">
@@ -3218,7 +3218,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>ethacrynic acid</t>
+          <t>3-Methyl-3H-imidazo[4,5-f]quinolin-2-amine</t>
         </is>
       </c>
       <c r="B279" t="n">
@@ -3228,7 +3228,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>Sucrose</t>
+          <t>Nicotinate, ethyl</t>
         </is>
       </c>
       <c r="B280" t="n">
@@ -3238,7 +3238,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>1-(diphenylmethyl)-4-ethylpiperazine</t>
+          <t>Benzene</t>
         </is>
       </c>
       <c r="B281" t="n">
@@ -3248,7 +3248,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>1-(diphenylmethyl)-4-methylpiperazine</t>
+          <t>Salicylic acid</t>
         </is>
       </c>
       <c r="B282" t="n">
@@ -3258,7 +3258,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>Methotrexate</t>
+          <t>Salicylic acid</t>
         </is>
       </c>
       <c r="B283" t="n">
@@ -3268,7 +3268,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>sucrose</t>
+          <t>benzoic acid</t>
         </is>
       </c>
       <c r="B284" t="n">
@@ -3278,7 +3278,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>Sucrose</t>
+          <t>Benzoic acid</t>
         </is>
       </c>
       <c r="B285" t="n">
@@ -3288,7 +3288,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>Benzoic acid</t>
         </is>
       </c>
       <c r="B286" t="n">
@@ -3298,7 +3298,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>1-(diphenylmethyl)-4-butylpiperazine</t>
+          <t>Caffeine</t>
         </is>
       </c>
       <c r="B287" t="n">
@@ -3308,7 +3308,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>Sotalol</t>
+          <t>Benzene</t>
         </is>
       </c>
       <c r="B288" t="n">
@@ -3318,7 +3318,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Sotalol</t>
+          <t>Naphthalene</t>
         </is>
       </c>
       <c r="B289" t="n">
@@ -3328,7 +3328,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>Nadolol</t>
+          <t>Nicotinate, ethyl</t>
         </is>
       </c>
       <c r="B290" t="n">
@@ -3338,7 +3338,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>Fentanyl base</t>
+          <t>4-Amino-3-nitrophenol</t>
         </is>
       </c>
       <c r="B291" t="n">
@@ -3348,7 +3348,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>Fentanyl base</t>
+          <t>Naphthol</t>
         </is>
       </c>
       <c r="B292" t="n">
@@ -3358,7 +3358,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>linolenic acid</t>
+          <t>Naphthol</t>
         </is>
       </c>
       <c r="B293" t="n">
@@ -3368,7 +3368,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>Estriol</t>
+          <t>Thymol; 2-Isopropyl-5-methylphenol</t>
         </is>
       </c>
       <c r="B294" t="n">
@@ -3378,7 +3378,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>Estriol</t>
+          <t>Thymol; 2-Isopropyl-5-methylphenol</t>
         </is>
       </c>
       <c r="B295" t="n">
@@ -3388,7 +3388,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>beta-Estradiol</t>
+          <t>o-t-butylphenol</t>
         </is>
       </c>
       <c r="B296" t="n">
@@ -3398,7 +3398,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>sotalol</t>
+          <t>2,4,6-Trichlorophenol</t>
         </is>
       </c>
       <c r="B297" t="n">
@@ -3408,7 +3408,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>beta-Estradiol</t>
+          <t>4-Amino-3-nitrophenol</t>
         </is>
       </c>
       <c r="B298" t="n">
@@ -3418,7 +3418,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>beta-Estradiol</t>
+          <t>chloroxylenol</t>
         </is>
       </c>
       <c r="B299" t="n">
@@ -3428,7 +3428,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>Beta-estradiol</t>
+          <t>pyrogallol</t>
         </is>
       </c>
       <c r="B300" t="n">
@@ -3438,7 +3438,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>beta-Estradiol</t>
+          <t>Diethyl phthalate</t>
         </is>
       </c>
       <c r="B301" t="n">
@@ -3448,7 +3448,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>chlorocresol</t>
         </is>
       </c>
       <c r="B302" t="n">
@@ -3458,7 +3458,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>chlorocresol</t>
         </is>
       </c>
       <c r="B303" t="n">
@@ -3468,7 +3468,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>2-Phenylethanol</t>
         </is>
       </c>
       <c r="B304" t="n">
@@ -3478,7 +3478,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>sotalol</t>
+          <t>2-phenylethanol</t>
         </is>
       </c>
       <c r="B305" t="n">
@@ -3488,7 +3488,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>Chloroxylenol</t>
         </is>
       </c>
       <c r="B306" t="n">
@@ -3498,7 +3498,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>sotalol</t>
+          <t>Caffeine</t>
         </is>
       </c>
       <c r="B307" t="n">
@@ -3508,7 +3508,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>oleic acid</t>
+          <t>p-Nitrophenol; 4-nitrophenol</t>
         </is>
       </c>
       <c r="B308" t="n">
@@ -3518,7 +3518,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>Atenolol</t>
+          <t>caffeine</t>
         </is>
       </c>
       <c r="B309" t="n">
@@ -3528,7 +3528,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>Timolol</t>
+          <t>2,4-dichlorophenol</t>
         </is>
       </c>
       <c r="B310" t="n">
@@ -3538,7 +3538,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>Timolol</t>
+          <t>2,4-dichlorophenol</t>
         </is>
       </c>
       <c r="B311" t="n">
@@ -3548,7 +3548,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>Naltrexone</t>
+          <t>2,4-dichlorophenol</t>
         </is>
       </c>
       <c r="B312" t="n">
@@ -3558,7 +3558,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>Lidocaine</t>
+          <t>Benzylideneacetone</t>
         </is>
       </c>
       <c r="B313" t="n">
@@ -3568,7 +3568,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>sotalol</t>
+          <t>Benzylideneacetone</t>
         </is>
       </c>
       <c r="B314" t="n">
@@ -3578,7 +3578,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>sotalol</t>
+          <t>p-Ethylphenol</t>
         </is>
       </c>
       <c r="B315" t="n">
@@ -3588,7 +3588,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>Lidocaine</t>
+          <t>Hydroquinone</t>
         </is>
       </c>
       <c r="B316" t="n">
@@ -3598,7 +3598,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>Lidocaine</t>
+          <t>hydroquinone</t>
         </is>
       </c>
       <c r="B317" t="n">
@@ -3608,7 +3608,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>Alprenolol</t>
+          <t>Hydroquinone</t>
         </is>
       </c>
       <c r="B318" t="n">
@@ -3618,7 +3618,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>Pindolol</t>
+          <t>Hydroquinone</t>
         </is>
       </c>
       <c r="B319" t="n">
@@ -3628,7 +3628,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>octylparaben</t>
+          <t>Dimethyl phthalate</t>
         </is>
       </c>
       <c r="B320" t="n">
@@ -3638,7 +3638,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>octylparaben</t>
+          <t>Dimethyl phthalate</t>
         </is>
       </c>
       <c r="B321" t="n">
@@ -3648,7 +3648,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>octylparaben</t>
+          <t>2,4-dichlorophenol</t>
         </is>
       </c>
       <c r="B322" t="n">
@@ -3658,7 +3658,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>octylparaben</t>
+          <t>Beta-naphthol; 2-naphthol</t>
         </is>
       </c>
       <c r="B323" t="n">
@@ -3668,7 +3668,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>octylparaben</t>
+          <t>Methyl 4-hydroxyphenylacetate</t>
         </is>
       </c>
       <c r="B324" t="n">
@@ -3678,7 +3678,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>bis(2-ethylhexyl)phthalate</t>
+          <t>trans-Cinnamaldehyde</t>
         </is>
       </c>
       <c r="B325" t="n">
@@ -3688,7 +3688,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>sotalol</t>
+          <t>trans-Cinnamaldehyde</t>
         </is>
       </c>
       <c r="B326" t="n">
@@ -3698,7 +3698,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>p-n-butylphenol; 4-Butylphenol</t>
         </is>
       </c>
       <c r="B327" t="n">
@@ -3708,7 +3708,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>Beta-estradiol</t>
+          <t>alfa-(4-Hydroxyphenyl) acetamide</t>
         </is>
       </c>
       <c r="B328" t="n">
@@ -3718,7 +3718,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>4-propoxyphenol</t>
         </is>
       </c>
       <c r="B329" t="n">
@@ -3728,7 +3728,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>Sufentanil base</t>
+          <t>4-propoxyphenol</t>
         </is>
       </c>
       <c r="B330" t="n">
@@ -3738,7 +3738,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>2-(Acetylamino)fluorene</t>
+          <t>4-Bromophenyl isocyanate</t>
         </is>
       </c>
       <c r="B331" t="n">
@@ -3748,7 +3748,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>2-(Acetylamino)fluorene</t>
+          <t>Caffeine</t>
         </is>
       </c>
       <c r="B332" t="n">
@@ -3758,7 +3758,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>Estrone</t>
+          <t>HC Red No. 3; 2-(4-Amino-2-nitroanilino)-ethanol</t>
         </is>
       </c>
       <c r="B333" t="n">
@@ -3768,7 +3768,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>Estrone</t>
+          <t>HC Red No. 3; 2-(4-Amino-2-nitroanilino)-ethanol</t>
         </is>
       </c>
       <c r="B334" t="n">
@@ -3778,7 +3778,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>Metoprolol</t>
+          <t>7-Ethoxycoumarin</t>
         </is>
       </c>
       <c r="B335" t="n">
@@ -3788,7 +3788,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>Beta-naphthol; 2-naphthol</t>
         </is>
       </c>
       <c r="B336" t="n">
@@ -3798,7 +3798,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>2,4-Dichlorophenol</t>
         </is>
       </c>
       <c r="B337" t="n">
@@ -3808,7 +3808,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>catechol</t>
         </is>
       </c>
       <c r="B338" t="n">
@@ -3818,7 +3818,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>Benzophenone</t>
         </is>
       </c>
       <c r="B339" t="n">
@@ -3828,7 +3828,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>Benzyl bromide</t>
         </is>
       </c>
       <c r="B340" t="n">
@@ -3838,7 +3838,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>Benzyl bromide</t>
         </is>
       </c>
       <c r="B341" t="n">
@@ -3848,7 +3848,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>Benzyl alcohol</t>
         </is>
       </c>
       <c r="B342" t="n">
@@ -3858,7 +3858,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>Cinnamyl alcohol</t>
         </is>
       </c>
       <c r="B343" t="n">
@@ -3868,7 +3868,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>Cinnamyl alcohol</t>
         </is>
       </c>
       <c r="B344" t="n">
@@ -3878,7 +3878,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>p-Tolunitrile</t>
         </is>
       </c>
       <c r="B345" t="n">
@@ -3888,7 +3888,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>Beta-Estradiol</t>
+          <t>p-Tolunitrile</t>
         </is>
       </c>
       <c r="B346" t="n">
@@ -3898,7 +3898,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>5-phenylpentanol</t>
         </is>
       </c>
       <c r="B347" t="n">
@@ -3908,7 +3908,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>p-Bromophenol</t>
         </is>
       </c>
       <c r="B348" t="n">
@@ -3918,7 +3918,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>p-Cresol</t>
         </is>
       </c>
       <c r="B349" t="n">
@@ -3928,7 +3928,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>p-Cresol</t>
         </is>
       </c>
       <c r="B350" t="n">
@@ -3938,7 +3938,7 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>p-Chlorophenol</t>
         </is>
       </c>
       <c r="B351" t="n">
@@ -3948,7 +3948,7 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>p-Phenylenediamine</t>
         </is>
       </c>
       <c r="B352" t="n">
@@ -3958,7 +3958,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>m-Cresol</t>
         </is>
       </c>
       <c r="B353" t="n">
@@ -3968,7 +3968,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>1-(diphenylmethyl)-4-propylpiperazine</t>
+          <t>Resorcinol; 1,3-Benzenediol</t>
         </is>
       </c>
       <c r="B354" t="n">
@@ -3978,7 +3978,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>resorcinol</t>
         </is>
       </c>
       <c r="B355" t="n">
@@ -3988,7 +3988,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>Resorcinol</t>
         </is>
       </c>
       <c r="B356" t="n">
@@ -3998,7 +3998,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>Resorcinol</t>
         </is>
       </c>
       <c r="B357" t="n">
@@ -4008,7 +4008,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>Estradiol</t>
+          <t>phloroglucinol</t>
         </is>
       </c>
       <c r="B358" t="n">
@@ -4018,7 +4018,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>Diazinon</t>
+          <t>Toluene</t>
         </is>
       </c>
       <c r="B359" t="n">
@@ -4028,407 +4028,407 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>decanol</t>
+          <t>Phenol</t>
         </is>
       </c>
       <c r="B360" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>Octanol</t>
+          <t>Phenol</t>
         </is>
       </c>
       <c r="B361" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>n-hexanol</t>
+          <t>Phenol</t>
         </is>
       </c>
       <c r="B362" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>Hexanol</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="B363" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>2-Ethoxy ethanol</t>
+          <t>4-Amino-2-Nitrophenol</t>
         </is>
       </c>
       <c r="B364" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>Diethyl maleate</t>
+          <t>methyl salicylate</t>
         </is>
       </c>
       <c r="B365" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>Diethyl maleate</t>
+          <t>Benzophenone</t>
         </is>
       </c>
       <c r="B366" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>Octanol</t>
+          <t>7-Ethoxycoumarin</t>
         </is>
       </c>
       <c r="B367" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>Nonanol</t>
+          <t>4-phenylbutanol</t>
         </is>
       </c>
       <c r="B368" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>Methylglucose</t>
+          <t>4-Bromophenyl isocyanate</t>
         </is>
       </c>
       <c r="B369" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>2-Butanone</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B370" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>Geraniol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B371" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>Geraniol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B372" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>2-Ethylhexyl acrylate</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B373" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>2-Ethylhexyl acrylate</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B374" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>n-nonanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B375" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>decanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B376" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>Octanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B377" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>decanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B378" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>butoxyethanol</t>
+          <t>5-Fluorouracil (+ - + -)</t>
         </is>
       </c>
       <c r="B379" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>decanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B380" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>Decanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B381" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>n-decanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B382" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>butoxyethanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B383" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t xml:space="preserve">Decanol </t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B384" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>Hexanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B385" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>Diethylene glycol monobutyl ether</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B386" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>decanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B387" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>Decanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B388" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>butoxyethanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B389" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>Octanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B390" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>n-octanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B391" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>butoxyethanol</t>
+          <t>5-Fluorouracil</t>
         </is>
       </c>
       <c r="B392" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>Diethylene glycol monobutyl ether</t>
+          <t>1,2,4-Benzenetriol</t>
         </is>
       </c>
       <c r="B393" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>butoxyethanol</t>
+          <t>2-(Acetylamino)fluorene</t>
         </is>
       </c>
       <c r="B394" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>Urea</t>
+          <t>Iso-thymol; Carvacrol</t>
         </is>
       </c>
       <c r="B395" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>Pentanol</t>
+          <t>2-(Acetylamino)fluorene</t>
         </is>
       </c>
       <c r="B396" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>Methyl methanesulfonate</t>
+          <t>m-Nitrophenol; 3-nitrophenol</t>
         </is>
       </c>
       <c r="B397" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>acetic acid</t>
+          <t>Caffeine</t>
         </is>
       </c>
       <c r="B398" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>acetic acid</t>
+          <t>Caffeine</t>
         </is>
       </c>
       <c r="B399" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>acetic acid</t>
+          <t>1-(diphenylmethyl)-4-ethylpiperazine</t>
         </is>
       </c>
       <c r="B400" t="n">
@@ -4438,7 +4438,7 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>acetic acid</t>
+          <t>bis(2-ethylhexyl)phthalate</t>
         </is>
       </c>
       <c r="B401" t="n">
@@ -4448,7 +4448,7 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>acetic acid</t>
+          <t>oleic acid</t>
         </is>
       </c>
       <c r="B402" t="n">
@@ -4458,7 +4458,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>Ethanol</t>
+          <t>1-(diphenylmethyl)-4-methylpiperazine</t>
         </is>
       </c>
       <c r="B403" t="n">
@@ -4468,7 +4468,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>ethanol</t>
+          <t>sucrose</t>
         </is>
       </c>
       <c r="B404" t="n">
@@ -4478,7 +4478,7 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>Ethanol</t>
+          <t>sucrose</t>
         </is>
       </c>
       <c r="B405" t="n">
@@ -4488,7 +4488,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>Cyclophosphamide monohydrate</t>
+          <t>Sucrose</t>
         </is>
       </c>
       <c r="B406" t="n">
@@ -4498,7 +4498,7 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>Methyl methanesulfonate</t>
+          <t>Raffinose</t>
         </is>
       </c>
       <c r="B407" t="n">
@@ -4508,7 +4508,7 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>Cyclophosphamide monohydrate</t>
+          <t>Methotrexate</t>
         </is>
       </c>
       <c r="B408" t="n">
@@ -4518,7 +4518,7 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>Heptanol</t>
+          <t>Raffinose</t>
         </is>
       </c>
       <c r="B409" t="n">
@@ -4528,7 +4528,7 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>Heptanol</t>
+          <t>Sucrose</t>
         </is>
       </c>
       <c r="B410" t="n">
@@ -4538,7 +4538,7 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>n-heptanol</t>
+          <t>Sucrose</t>
         </is>
       </c>
       <c r="B411" t="n">
@@ -4548,7 +4548,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>Glycerol</t>
+          <t>Sucrose</t>
         </is>
       </c>
       <c r="B412" t="n">
@@ -4558,7 +4558,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>Glycerol</t>
+          <t>Sucrose</t>
         </is>
       </c>
       <c r="B413" t="n">
@@ -4568,7 +4568,7 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>urea</t>
+          <t>Sufentanil base</t>
         </is>
       </c>
       <c r="B414" t="n">
@@ -4578,7 +4578,7 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>urea</t>
+          <t>Metoprolol</t>
         </is>
       </c>
       <c r="B415" t="n">
@@ -4588,7 +4588,7 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>Urea</t>
+          <t>Methotrexate</t>
         </is>
       </c>
       <c r="B416" t="n">
@@ -4598,7 +4598,7 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>Urea</t>
+          <t>ethacrynic acid</t>
         </is>
       </c>
       <c r="B417" t="n">
@@ -4608,7 +4608,7 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>Urea</t>
+          <t>Diazinon</t>
         </is>
       </c>
       <c r="B418" t="n">
@@ -4618,7 +4618,7 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>2,3-Butanediol</t>
+          <t>Cyclophosphamide monohydrate</t>
         </is>
       </c>
       <c r="B419" t="n">
@@ -4628,7 +4628,7 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>Methanol</t>
+          <t>sotalol</t>
         </is>
       </c>
       <c r="B420" t="n">
@@ -4638,7 +4638,7 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>Methanol</t>
+          <t>sotalol</t>
         </is>
       </c>
       <c r="B421" t="n">
@@ -4648,7 +4648,7 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>methanol</t>
+          <t>Atenolol</t>
         </is>
       </c>
       <c r="B422" t="n">
@@ -4658,7 +4658,7 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>Butanol</t>
+          <t>sotalol</t>
         </is>
       </c>
       <c r="B423" t="n">
@@ -4668,7 +4668,7 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>n-butanol</t>
+          <t>sotalol</t>
         </is>
       </c>
       <c r="B424" t="n">
@@ -4678,7 +4678,7 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>Butanol</t>
+          <t>Timolol</t>
         </is>
       </c>
       <c r="B425" t="n">
@@ -4688,7 +4688,7 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>Butanol</t>
+          <t>Timolol</t>
         </is>
       </c>
       <c r="B426" t="n">
@@ -4698,7 +4698,7 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>Butanol</t>
+          <t>sotalol</t>
         </is>
       </c>
       <c r="B427" t="n">
@@ -4708,7 +4708,7 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>Butanol</t>
+          <t>Sotalol</t>
         </is>
       </c>
       <c r="B428" t="n">
@@ -4718,7 +4718,7 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>n-propanol</t>
+          <t>Sotalol</t>
         </is>
       </c>
       <c r="B429" t="n">
@@ -4728,7 +4728,7 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>Propanol</t>
+          <t>Nadolol</t>
         </is>
       </c>
       <c r="B430" t="n">
@@ -4738,7 +4738,7 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>Propanol</t>
+          <t>Fentanyl base</t>
         </is>
       </c>
       <c r="B431" t="n">
@@ -4748,7 +4748,7 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>Cyclophosphamide monohydrate</t>
         </is>
       </c>
       <c r="B432" t="n">
@@ -4758,7 +4758,7 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>Fentanyl base</t>
         </is>
       </c>
       <c r="B433" t="n">
@@ -4768,7 +4768,7 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>1-(diphenylmethyl)-4-propylpiperazine</t>
         </is>
       </c>
       <c r="B434" t="n">
@@ -4778,7 +4778,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>Lidocaine</t>
         </is>
       </c>
       <c r="B435" t="n">
@@ -4788,7 +4788,7 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>Lidocaine</t>
         </is>
       </c>
       <c r="B436" t="n">
@@ -4798,7 +4798,7 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>Lidocaine</t>
         </is>
       </c>
       <c r="B437" t="n">
@@ -4808,7 +4808,7 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>Alprenolol</t>
         </is>
       </c>
       <c r="B438" t="n">
@@ -4818,7 +4818,7 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>Pindolol</t>
         </is>
       </c>
       <c r="B439" t="n">
@@ -4828,7 +4828,7 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>octylparaben</t>
         </is>
       </c>
       <c r="B440" t="n">
@@ -4838,7 +4838,7 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>octylparaben</t>
         </is>
       </c>
       <c r="B441" t="n">
@@ -4848,7 +4848,7 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>octylparaben</t>
         </is>
       </c>
       <c r="B442" t="n">
@@ -4858,7 +4858,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>octylparaben</t>
         </is>
       </c>
       <c r="B443" t="n">
@@ -4868,7 +4868,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>Urea</t>
+          <t>octylparaben</t>
         </is>
       </c>
       <c r="B444" t="n">
@@ -4878,7 +4878,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>Ethyl ether</t>
+          <t>sotalol</t>
         </is>
       </c>
       <c r="B445" t="n">
@@ -4888,7 +4888,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>n-pentanol</t>
+          <t>linolenic acid</t>
         </is>
       </c>
       <c r="B446" t="n">
@@ -4898,7 +4898,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>Mannitol</t>
+          <t>1-(diphenylmethyl)-4-butylpiperazine</t>
         </is>
       </c>
       <c r="B447" t="n">

</xml_diff>